<commit_message>
aula 3 - notas e modelos de regressões
</commit_message>
<xml_diff>
--- a/PIBIU_PT_SETEMBRO23_3.xlsx
+++ b/PIBIU_PT_SETEMBRO23_3.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogenesjusto/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giossaurus/Developer/BigDataScienceFIAP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C39A96C7-66E0-4342-9681-E0A3C33FA0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007882A0-C051-FD44-9BA5-6A6C0CB2F936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6440" yWindow="2180" windowWidth="22960" windowHeight="19360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RLS_BRL" sheetId="3" r:id="rId1"/>
     <sheet name="PM-Itaú" sheetId="1" r:id="rId2"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId3"/>
+    <sheet name="Dados AR" sheetId="4" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>PIB</t>
   </si>
@@ -162,6 +163,45 @@
   <si>
     <t>PIB = 0,51*BRL+66,45</t>
   </si>
+  <si>
+    <t>jan.-22</t>
+  </si>
+  <si>
+    <t>fev.-22</t>
+  </si>
+  <si>
+    <t>A1*SPP(JAN22) + A2*SPT(JAN22)+B</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y(i-2)</t>
+  </si>
+  <si>
+    <t>y(i-1)</t>
+  </si>
+  <si>
+    <t>PIB(1)</t>
+  </si>
+  <si>
+    <t>PIB(i-1)</t>
+  </si>
+  <si>
+    <t>PIB(i-2)</t>
+  </si>
+  <si>
+    <t>PIBi1</t>
+  </si>
+  <si>
+    <t>PIBi2</t>
+  </si>
+  <si>
+    <t>nulo</t>
+  </si>
 </sst>
 </file>
 
@@ -181,7 +221,7 @@
     <numFmt numFmtId="173" formatCode="0.00\ %"/>
     <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +291,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -369,7 +417,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,6 +459,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -442,6 +505,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -456,7 +524,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -493,7 +561,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -660,7 +728,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="58218576"/>
@@ -722,7 +790,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1818521584"/>
@@ -770,7 +838,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1667,7 +1735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DEF39E-E74E-124B-92B4-A03C86A91373}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1905,13 +1973,14 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B225" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="H232" sqref="H232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="7.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="3" customWidth="1"/>
+    <col min="3" max="14" width="7.5" style="3" customWidth="1"/>
     <col min="15" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
@@ -12042,1060 +12111,482 @@
       </c>
     </row>
     <row r="232" spans="1:14" ht="15">
-      <c r="C232" s="9">
-        <v>156.85784454988806</v>
-      </c>
-      <c r="D232" s="10">
-        <v>148.11748491537716</v>
-      </c>
-      <c r="E232" s="11">
-        <v>154.85422202009534</v>
-      </c>
-      <c r="F232" s="9">
-        <v>155.32559080947985</v>
-      </c>
-      <c r="G232" s="10">
-        <v>161.19028837109369</v>
-      </c>
-      <c r="H232" s="11">
-        <v>155.47880974763416</v>
+      <c r="A232" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C232" s="9"/>
+      <c r="D232" s="10"/>
+      <c r="E232" s="11"/>
+      <c r="F232" s="9"/>
+      <c r="G232" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H232" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="I232" s="9"/>
       <c r="J232" s="10"/>
       <c r="K232" s="11"/>
-      <c r="L232" s="9">
-        <v>135.3677075363623</v>
-      </c>
-      <c r="M232" s="10">
-        <v>111.13894359302617</v>
-      </c>
-      <c r="N232" s="11">
-        <v>131.44868060477563</v>
-      </c>
+      <c r="L232" s="9"/>
+      <c r="M232" s="10"/>
+      <c r="N232" s="11"/>
     </row>
     <row r="233" spans="1:14" ht="15">
-      <c r="C233" s="9">
-        <v>138.82488507603969</v>
-      </c>
-      <c r="D233" s="10">
-        <v>149.16581200104139</v>
-      </c>
-      <c r="E233" s="11">
-        <v>140.96114731475365</v>
-      </c>
-      <c r="F233" s="9">
-        <v>141.25154111347874</v>
-      </c>
-      <c r="G233" s="10">
-        <v>163.99045257533973</v>
-      </c>
-      <c r="H233" s="11">
-        <v>145.48480978202559</v>
-      </c>
+      <c r="A233" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C233" s="9"/>
+      <c r="D233" s="10"/>
+      <c r="E233" s="11"/>
+      <c r="F233" s="9"/>
+      <c r="G233" s="10"/>
+      <c r="H233" s="11"/>
       <c r="I233" s="9"/>
       <c r="J233" s="10"/>
       <c r="K233" s="11"/>
-      <c r="L233" s="9">
-        <v>117.57092423867127</v>
-      </c>
-      <c r="M233" s="10">
-        <v>106.60096861934836</v>
-      </c>
-      <c r="N233" s="11">
-        <v>115.89998108018965</v>
-      </c>
+      <c r="L233" s="9"/>
+      <c r="M233" s="10"/>
+      <c r="N233" s="11"/>
     </row>
     <row r="234" spans="1:14" ht="15">
-      <c r="C234" s="9">
-        <v>152.12480666383368</v>
-      </c>
-      <c r="D234" s="10">
-        <v>170.29743260591638</v>
-      </c>
-      <c r="E234" s="11">
-        <v>155.35697131347467</v>
-      </c>
-      <c r="F234" s="9">
-        <v>158.71462010628625</v>
-      </c>
-      <c r="G234" s="10">
-        <v>188.35111467858027</v>
-      </c>
-      <c r="H234" s="11">
-        <v>164.21525576324734</v>
-      </c>
+      <c r="C234" s="9"/>
+      <c r="D234" s="10"/>
+      <c r="E234" s="11"/>
+      <c r="F234" s="9"/>
+      <c r="G234" s="10"/>
+      <c r="H234" s="11"/>
       <c r="I234" s="9"/>
       <c r="J234" s="10"/>
       <c r="K234" s="11"/>
-      <c r="L234" s="9">
-        <v>140.87041391460303</v>
-      </c>
-      <c r="M234" s="10">
-        <v>120.71791053414464</v>
-      </c>
-      <c r="N234" s="11">
-        <v>137.06863955944632</v>
-      </c>
+      <c r="L234" s="9"/>
+      <c r="M234" s="10"/>
+      <c r="N234" s="11"/>
     </row>
     <row r="235" spans="1:14" ht="15">
-      <c r="C235" s="9">
-        <v>149.67722529497996</v>
-      </c>
-      <c r="D235" s="10">
-        <v>157.52710367867272</v>
-      </c>
-      <c r="E235" s="11">
-        <v>150.78030682028592</v>
-      </c>
-      <c r="F235" s="9">
-        <v>159.46177559281719</v>
-      </c>
-      <c r="G235" s="10">
-        <v>172.98545544945063</v>
-      </c>
-      <c r="H235" s="11">
-        <v>161.58454163132643</v>
-      </c>
+      <c r="C235" s="9"/>
+      <c r="D235" s="10"/>
+      <c r="E235" s="11"/>
+      <c r="F235" s="9"/>
+      <c r="G235" s="10"/>
+      <c r="H235" s="11"/>
       <c r="I235" s="9"/>
       <c r="J235" s="10"/>
       <c r="K235" s="11"/>
-      <c r="L235" s="9">
-        <v>131.40117284095126</v>
-      </c>
-      <c r="M235" s="10">
-        <v>109.80544851243067</v>
-      </c>
-      <c r="N235" s="11">
-        <v>127.66759063966205</v>
-      </c>
+      <c r="L235" s="9"/>
+      <c r="M235" s="10"/>
+      <c r="N235" s="11"/>
     </row>
     <row r="236" spans="1:14" ht="15">
-      <c r="C236" s="9">
-        <v>144.40219428868971</v>
-      </c>
-      <c r="D236" s="10">
-        <v>170.06118347341553</v>
-      </c>
-      <c r="E236" s="11">
-        <v>149.72431729045891</v>
-      </c>
-      <c r="F236" s="9">
-        <v>157.10637741218349</v>
-      </c>
-      <c r="G236" s="10">
-        <v>194.98507936032351</v>
-      </c>
-      <c r="H236" s="11">
-        <v>164.06073830597751</v>
-      </c>
+      <c r="C236" s="9"/>
+      <c r="D236" s="10"/>
+      <c r="E236" s="11"/>
+      <c r="F236" s="9"/>
+      <c r="G236" s="10"/>
+      <c r="H236" s="11"/>
       <c r="I236" s="9"/>
       <c r="J236" s="10"/>
       <c r="K236" s="11"/>
-      <c r="L236" s="9">
-        <v>132.039568301012</v>
-      </c>
-      <c r="M236" s="10">
-        <v>118.48042034399164</v>
-      </c>
-      <c r="N236" s="11">
-        <v>130.09244286199123</v>
-      </c>
+      <c r="L236" s="9"/>
+      <c r="M236" s="10"/>
+      <c r="N236" s="11"/>
     </row>
     <row r="237" spans="1:14" ht="15">
-      <c r="C237" s="9">
-        <v>137.34009610302144</v>
-      </c>
-      <c r="D237" s="10">
-        <v>162.25885261108459</v>
-      </c>
-      <c r="E237" s="11">
-        <v>142.59452883745382</v>
-      </c>
-      <c r="F237" s="9">
-        <v>143.53083399716306</v>
-      </c>
-      <c r="G237" s="10">
-        <v>181.48006650325547</v>
-      </c>
-      <c r="H237" s="11">
-        <v>150.57636602733609</v>
-      </c>
+      <c r="C237" s="9"/>
+      <c r="D237" s="10"/>
+      <c r="E237" s="11"/>
+      <c r="F237" s="9"/>
+      <c r="G237" s="10"/>
+      <c r="H237" s="11"/>
       <c r="I237" s="9"/>
       <c r="J237" s="10"/>
       <c r="K237" s="11"/>
-      <c r="L237" s="9">
-        <v>123.78321214938202</v>
-      </c>
-      <c r="M237" s="10">
-        <v>111.03901833102688</v>
-      </c>
-      <c r="N237" s="11">
-        <v>121.4413078444697</v>
-      </c>
+      <c r="L237" s="9"/>
+      <c r="M237" s="10"/>
+      <c r="N237" s="11"/>
     </row>
     <row r="238" spans="1:14" ht="15">
-      <c r="C238" s="9">
-        <v>162.96549524107252</v>
-      </c>
-      <c r="D238" s="10">
-        <v>169.17117835197507</v>
-      </c>
-      <c r="E238" s="11">
-        <v>163.94662265173633</v>
-      </c>
-      <c r="F238" s="9">
-        <v>172.15300038984586</v>
-      </c>
-      <c r="G238" s="10">
-        <v>188.43318050273729</v>
-      </c>
-      <c r="H238" s="11">
-        <v>174.60756396548624</v>
-      </c>
+      <c r="C238" s="9"/>
+      <c r="D238" s="10"/>
+      <c r="E238" s="11"/>
+      <c r="F238" s="9"/>
+      <c r="G238" s="10"/>
+      <c r="H238" s="11"/>
       <c r="I238" s="9"/>
       <c r="J238" s="10"/>
       <c r="K238" s="11"/>
-      <c r="L238" s="9">
-        <v>143.07639392183663</v>
-      </c>
-      <c r="M238" s="10">
-        <v>114.39771803405297</v>
-      </c>
-      <c r="N238" s="11">
-        <v>137.96913095437549</v>
-      </c>
+      <c r="L238" s="9"/>
+      <c r="M238" s="10"/>
+      <c r="N238" s="11"/>
     </row>
     <row r="239" spans="1:14" ht="15">
-      <c r="C239" s="9">
-        <v>151.00402399667379</v>
-      </c>
-      <c r="D239" s="10">
-        <v>173.31076115876914</v>
-      </c>
-      <c r="E239" s="11">
-        <v>155.63077521394197</v>
-      </c>
-      <c r="F239" s="9">
-        <v>160.04013074780008</v>
-      </c>
-      <c r="G239" s="10">
-        <v>195.0799256543425</v>
-      </c>
-      <c r="H239" s="11">
-        <v>166.97965605763849</v>
-      </c>
+      <c r="C239" s="9"/>
+      <c r="D239" s="10"/>
+      <c r="E239" s="11"/>
+      <c r="F239" s="9"/>
+      <c r="G239" s="10"/>
+      <c r="H239" s="11"/>
       <c r="I239" s="9"/>
       <c r="J239" s="10"/>
       <c r="K239" s="11"/>
-      <c r="L239" s="9">
-        <v>135.36896248132817</v>
-      </c>
-      <c r="M239" s="10">
-        <v>116.87488824275634</v>
-      </c>
-      <c r="N239" s="11">
-        <v>132.01818351275114</v>
-      </c>
+      <c r="L239" s="9"/>
+      <c r="M239" s="10"/>
+      <c r="N239" s="11"/>
     </row>
     <row r="240" spans="1:14" ht="15">
-      <c r="C240" s="9">
-        <v>151.0109261421496</v>
-      </c>
-      <c r="D240" s="10">
-        <v>166.28211404713639</v>
-      </c>
-      <c r="E240" s="11">
-        <v>153.99535413411382</v>
-      </c>
-      <c r="F240" s="9">
-        <v>159.03108494153</v>
-      </c>
-      <c r="G240" s="10">
-        <v>187.2224226529965</v>
-      </c>
-      <c r="H240" s="11">
-        <v>164.77740530217625</v>
-      </c>
+      <c r="C240" s="9"/>
+      <c r="D240" s="10"/>
+      <c r="E240" s="11"/>
+      <c r="F240" s="9"/>
+      <c r="G240" s="10"/>
+      <c r="H240" s="11"/>
       <c r="I240" s="9"/>
       <c r="J240" s="10"/>
       <c r="K240" s="11"/>
-      <c r="L240" s="9">
-        <v>136.38738074594986</v>
-      </c>
-      <c r="M240" s="10">
-        <v>117.15266191118542</v>
-      </c>
-      <c r="N240" s="11">
-        <v>132.862712634259</v>
-      </c>
+      <c r="L240" s="9"/>
+      <c r="M240" s="10"/>
+      <c r="N240" s="11"/>
     </row>
     <row r="241" spans="3:14" ht="15">
-      <c r="C241" s="9">
-        <v>157.20174227399517</v>
-      </c>
-      <c r="D241" s="10">
-        <v>164.68032310392778</v>
-      </c>
-      <c r="E241" s="11">
-        <v>158.38619863118265</v>
-      </c>
-      <c r="F241" s="9">
-        <v>166.46614845770816</v>
-      </c>
-      <c r="G241" s="10">
-        <v>185.07100873055001</v>
-      </c>
-      <c r="H241" s="11">
-        <v>169.33925262853623</v>
-      </c>
+      <c r="C241" s="9"/>
+      <c r="D241" s="10"/>
+      <c r="E241" s="11"/>
+      <c r="F241" s="9"/>
+      <c r="G241" s="10"/>
+      <c r="H241" s="11"/>
       <c r="I241" s="9"/>
       <c r="J241" s="10"/>
       <c r="K241" s="11"/>
-      <c r="L241" s="9">
-        <v>140.2850422452133</v>
-      </c>
-      <c r="M241" s="10">
-        <v>112.02108861763556</v>
-      </c>
-      <c r="N241" s="11">
-        <v>135.05223354200066</v>
-      </c>
+      <c r="L241" s="9"/>
+      <c r="M241" s="10"/>
+      <c r="N241" s="11"/>
     </row>
     <row r="242" spans="3:14" ht="15">
-      <c r="C242" s="9">
-        <v>149.58097443919075</v>
-      </c>
-      <c r="D242" s="10">
-        <v>160.28018582041466</v>
-      </c>
-      <c r="E242" s="11">
-        <v>151.54077531017262</v>
-      </c>
-      <c r="F242" s="9">
-        <v>156.97125994114268</v>
-      </c>
-      <c r="G242" s="10">
-        <v>181.47534237684124</v>
-      </c>
-      <c r="H242" s="11">
-        <v>161.36515365335788</v>
-      </c>
+      <c r="C242" s="9"/>
+      <c r="D242" s="10"/>
+      <c r="E242" s="11"/>
+      <c r="F242" s="9"/>
+      <c r="G242" s="10"/>
+      <c r="H242" s="11"/>
       <c r="I242" s="9"/>
       <c r="J242" s="10"/>
       <c r="K242" s="11"/>
-      <c r="L242" s="9">
-        <v>133.01007837076949</v>
-      </c>
-      <c r="M242" s="10">
-        <v>114.9630147358498</v>
-      </c>
-      <c r="N242" s="11">
-        <v>129.8084492267983</v>
-      </c>
+      <c r="L242" s="9"/>
+      <c r="M242" s="10"/>
+      <c r="N242" s="11"/>
     </row>
     <row r="243" spans="3:14" ht="15">
-      <c r="C243" s="9">
-        <v>177.10747048935008</v>
-      </c>
-      <c r="D243" s="10">
-        <v>155.54673456526498</v>
-      </c>
-      <c r="E243" s="11">
-        <v>171.71072346891603</v>
-      </c>
-      <c r="F243" s="9">
-        <v>184.85697949765824</v>
-      </c>
-      <c r="G243" s="10">
-        <v>174.80027370744591</v>
-      </c>
-      <c r="H243" s="11">
-        <v>181.54192218346128</v>
-      </c>
+      <c r="C243" s="9"/>
+      <c r="D243" s="10"/>
+      <c r="E243" s="11"/>
+      <c r="F243" s="9"/>
+      <c r="G243" s="10"/>
+      <c r="H243" s="11"/>
       <c r="I243" s="9"/>
       <c r="J243" s="10"/>
       <c r="K243" s="11"/>
-      <c r="L243" s="9">
-        <v>150.46829856604037</v>
-      </c>
-      <c r="M243" s="10">
-        <v>113.94545949297469</v>
-      </c>
-      <c r="N243" s="11">
-        <v>144.04330051624865</v>
-      </c>
+      <c r="L243" s="9"/>
+      <c r="M243" s="10"/>
+      <c r="N243" s="11"/>
     </row>
     <row r="244" spans="3:14" ht="15">
-      <c r="C244" s="9">
-        <v>180.92103060545944</v>
-      </c>
-      <c r="D244" s="10">
-        <v>151.6153763841794</v>
-      </c>
-      <c r="E244" s="11">
-        <v>173.89425918822801</v>
-      </c>
-      <c r="F244" s="9">
-        <v>181.85702248942772</v>
-      </c>
-      <c r="G244" s="10">
-        <v>166.03340970894959</v>
-      </c>
-      <c r="H244" s="11">
-        <v>177.26297108084611</v>
-      </c>
+      <c r="C244" s="9"/>
+      <c r="D244" s="10"/>
+      <c r="E244" s="11"/>
+      <c r="F244" s="9"/>
+      <c r="G244" s="10"/>
+      <c r="H244" s="11"/>
       <c r="I244" s="9"/>
       <c r="J244" s="10"/>
       <c r="K244" s="11"/>
-      <c r="L244" s="9">
-        <v>149.24677110642432</v>
-      </c>
-      <c r="M244" s="10">
-        <v>112.81941351760871</v>
-      </c>
-      <c r="N244" s="11">
-        <v>143.0845961489008</v>
-      </c>
+      <c r="L244" s="9"/>
+      <c r="M244" s="10"/>
+      <c r="N244" s="11"/>
     </row>
     <row r="245" spans="3:14" ht="15">
-      <c r="C245" s="9">
-        <v>148.81080276887883</v>
-      </c>
-      <c r="D245" s="10">
-        <v>145.23107923754446</v>
-      </c>
-      <c r="E245" s="11">
-        <v>147.54315459732081</v>
-      </c>
-      <c r="F245" s="9">
-        <v>150.87087399591411</v>
-      </c>
-      <c r="G245" s="10">
-        <v>160.09555697471902</v>
-      </c>
-      <c r="H245" s="11">
-        <v>152.24737538038252</v>
-      </c>
+      <c r="C245" s="9"/>
+      <c r="D245" s="10"/>
+      <c r="E245" s="11"/>
+      <c r="F245" s="9"/>
+      <c r="G245" s="10"/>
+      <c r="H245" s="11"/>
       <c r="I245" s="9"/>
       <c r="J245" s="10"/>
       <c r="K245" s="11"/>
-      <c r="L245" s="9">
-        <v>124.89516406921581</v>
-      </c>
-      <c r="M245" s="10">
-        <v>102.74716896574924</v>
-      </c>
-      <c r="N245" s="11">
-        <v>121.15255949032706</v>
-      </c>
+      <c r="L245" s="9"/>
+      <c r="M245" s="10"/>
+      <c r="N245" s="11"/>
     </row>
     <row r="246" spans="3:14" ht="15">
-      <c r="C246" s="9">
-        <v>160.17135010561537</v>
-      </c>
-      <c r="D246" s="10">
-        <v>175.77810859268826</v>
-      </c>
-      <c r="E246" s="11">
-        <v>162.73263259287782</v>
-      </c>
-      <c r="F246" s="9">
-        <v>168.81258754284411</v>
-      </c>
-      <c r="G246" s="10">
-        <v>195.23044190111355</v>
-      </c>
-      <c r="H246" s="11">
-        <v>173.59712817190965</v>
-      </c>
+      <c r="C246" s="9"/>
+      <c r="D246" s="10"/>
+      <c r="E246" s="11"/>
+      <c r="F246" s="9"/>
+      <c r="G246" s="10"/>
+      <c r="H246" s="11"/>
       <c r="I246" s="9"/>
       <c r="J246" s="10"/>
       <c r="K246" s="11"/>
-      <c r="L246" s="9">
-        <v>140.63590813877022</v>
-      </c>
-      <c r="M246" s="10">
-        <v>125.3409674316274</v>
-      </c>
-      <c r="N246" s="11">
-        <v>137.77760500338164</v>
-      </c>
+      <c r="L246" s="9"/>
+      <c r="M246" s="10"/>
+      <c r="N246" s="11"/>
     </row>
     <row r="247" spans="3:14" ht="15">
-      <c r="C247" s="9">
-        <v>158.04053439426275</v>
-      </c>
-      <c r="D247" s="10">
-        <v>154.59482016243095</v>
-      </c>
-      <c r="E247" s="11">
-        <v>156.43980824605001</v>
-      </c>
-      <c r="F247" s="9">
-        <v>168.80061095391628</v>
-      </c>
-      <c r="G247" s="10">
-        <v>170.49804990568475</v>
-      </c>
-      <c r="H247" s="11">
-        <v>168.42418003304903</v>
-      </c>
+      <c r="C247" s="9"/>
+      <c r="D247" s="10"/>
+      <c r="E247" s="11"/>
+      <c r="F247" s="9"/>
+      <c r="G247" s="10"/>
+      <c r="H247" s="11"/>
       <c r="I247" s="9"/>
       <c r="J247" s="10"/>
       <c r="K247" s="11"/>
-      <c r="L247" s="9">
-        <v>136.12333413130889</v>
-      </c>
-      <c r="M247" s="10">
-        <v>106.62407467585282</v>
-      </c>
-      <c r="N247" s="11">
-        <v>130.84236971931227</v>
-      </c>
+      <c r="L247" s="9"/>
+      <c r="M247" s="10"/>
+      <c r="N247" s="11"/>
     </row>
     <row r="248" spans="3:14" ht="15">
-      <c r="C248" s="9">
-        <v>154.76360838845994</v>
-      </c>
-      <c r="D248" s="10">
-        <v>174.08444927636955</v>
-      </c>
-      <c r="E248" s="11">
-        <v>158.54029541662021</v>
-      </c>
-      <c r="F248" s="9">
-        <v>168.90031231942109</v>
-      </c>
-      <c r="G248" s="10">
-        <v>201.88703286712263</v>
-      </c>
-      <c r="H248" s="11">
-        <v>174.79592711638361</v>
-      </c>
+      <c r="C248" s="9"/>
+      <c r="D248" s="10"/>
+      <c r="E248" s="11"/>
+      <c r="F248" s="9"/>
+      <c r="G248" s="10"/>
+      <c r="H248" s="11"/>
       <c r="I248" s="9"/>
       <c r="J248" s="10"/>
       <c r="K248" s="11"/>
-      <c r="L248" s="9">
-        <v>138.77935270109234</v>
-      </c>
-      <c r="M248" s="10">
-        <v>118.69450228224935</v>
-      </c>
-      <c r="N248" s="11">
-        <v>135.57627027896368</v>
-      </c>
+      <c r="L248" s="9"/>
+      <c r="M248" s="10"/>
+      <c r="N248" s="11"/>
     </row>
     <row r="249" spans="3:14" ht="15">
-      <c r="C249" s="9">
-        <v>151.06967253757631</v>
-      </c>
-      <c r="D249" s="10">
-        <v>165.64610874717133</v>
-      </c>
-      <c r="E249" s="11">
-        <v>153.83768600351684</v>
-      </c>
-      <c r="F249" s="9">
-        <v>158.22616682812756</v>
-      </c>
-      <c r="G249" s="10">
-        <v>185.7312560036778</v>
-      </c>
-      <c r="H249" s="11">
-        <v>163.08620908527053</v>
-      </c>
+      <c r="C249" s="9"/>
+      <c r="D249" s="10"/>
+      <c r="E249" s="11"/>
+      <c r="F249" s="9"/>
+      <c r="G249" s="10"/>
+      <c r="H249" s="11"/>
       <c r="I249" s="9"/>
       <c r="J249" s="10"/>
       <c r="K249" s="11"/>
-      <c r="L249" s="9">
-        <v>135.75551313015495</v>
-      </c>
-      <c r="M249" s="10">
-        <v>112.42403157544</v>
-      </c>
-      <c r="N249" s="11">
-        <v>131.3297757250771</v>
-      </c>
+      <c r="L249" s="9"/>
+      <c r="M249" s="10"/>
+      <c r="N249" s="11"/>
     </row>
     <row r="250" spans="3:14" ht="15">
-      <c r="C250" s="9">
-        <v>170.28338558524132</v>
-      </c>
-      <c r="D250" s="10">
-        <v>173.36853883626364</v>
-      </c>
-      <c r="E250" s="11">
-        <v>170.50576436147247</v>
-      </c>
-      <c r="F250" s="9">
-        <v>179.74591131826699</v>
-      </c>
-      <c r="G250" s="10">
-        <v>193.7698015969718</v>
-      </c>
-      <c r="H250" s="11">
-        <v>181.69782602358461</v>
-      </c>
+      <c r="C250" s="9"/>
+      <c r="D250" s="10"/>
+      <c r="E250" s="11"/>
+      <c r="F250" s="9"/>
+      <c r="G250" s="10"/>
+      <c r="H250" s="11"/>
       <c r="I250" s="9"/>
       <c r="J250" s="10"/>
       <c r="K250" s="11"/>
-      <c r="L250" s="9">
-        <v>146.38924354806136</v>
-      </c>
-      <c r="M250" s="10">
-        <v>116.97666212239764</v>
-      </c>
-      <c r="N250" s="11">
-        <v>141.15008218382457</v>
-      </c>
+      <c r="L250" s="9"/>
+      <c r="M250" s="10"/>
+      <c r="N250" s="11"/>
     </row>
     <row r="251" spans="3:14" ht="15">
-      <c r="C251" s="9">
-        <v>157.67537112512258</v>
-      </c>
-      <c r="D251" s="10">
-        <v>181.14344958985552</v>
-      </c>
-      <c r="E251" s="11">
-        <v>162.54829630558734</v>
-      </c>
-      <c r="F251" s="9">
-        <v>167.96772607345497</v>
-      </c>
-      <c r="G251" s="10">
-        <v>203.65883270861559</v>
-      </c>
-      <c r="H251" s="11">
-        <v>175.0275290661283</v>
-      </c>
+      <c r="C251" s="9"/>
+      <c r="D251" s="10"/>
+      <c r="E251" s="11"/>
+      <c r="F251" s="9"/>
+      <c r="G251" s="10"/>
+      <c r="H251" s="11"/>
       <c r="I251" s="9"/>
       <c r="J251" s="10"/>
       <c r="K251" s="11"/>
-      <c r="L251" s="9">
-        <v>139.32814921828393</v>
-      </c>
-      <c r="M251" s="10">
-        <v>121.89442422523442</v>
-      </c>
-      <c r="N251" s="11">
-        <v>136.2007044127763</v>
-      </c>
+      <c r="L251" s="9"/>
+      <c r="M251" s="10"/>
+      <c r="N251" s="11"/>
     </row>
     <row r="252" spans="3:14" ht="15">
-      <c r="C252" s="9">
-        <v>163.35226536057493</v>
-      </c>
-      <c r="D252" s="10">
-        <v>171.63099392647922</v>
-      </c>
-      <c r="E252" s="11">
-        <v>164.61320327688233</v>
-      </c>
-      <c r="F252" s="9">
-        <v>173.59497112805644</v>
-      </c>
-      <c r="G252" s="10">
-        <v>193.844981152814</v>
-      </c>
-      <c r="H252" s="11">
-        <v>177.69636816141781</v>
-      </c>
+      <c r="C252" s="9"/>
+      <c r="D252" s="10"/>
+      <c r="E252" s="11"/>
+      <c r="F252" s="9"/>
+      <c r="G252" s="10"/>
+      <c r="H252" s="11"/>
       <c r="I252" s="9"/>
       <c r="J252" s="10"/>
       <c r="K252" s="11"/>
-      <c r="L252" s="9">
-        <v>145.50672478492481</v>
-      </c>
-      <c r="M252" s="10">
-        <v>121.47659510244463</v>
-      </c>
-      <c r="N252" s="11">
-        <v>141.05625354800975</v>
-      </c>
+      <c r="L252" s="9"/>
+      <c r="M252" s="10"/>
+      <c r="N252" s="11"/>
     </row>
     <row r="253" spans="3:14" ht="15">
-      <c r="C253" s="9">
-        <v>161.86291452198498</v>
-      </c>
-      <c r="D253" s="10">
-        <v>177.21201265213122</v>
-      </c>
-      <c r="E253" s="11">
-        <v>164.90846981999388</v>
-      </c>
-      <c r="F253" s="9">
-        <v>172.00712372354505</v>
-      </c>
-      <c r="G253" s="10">
-        <v>198.48039439573415</v>
-      </c>
-      <c r="H253" s="11">
-        <v>176.46997104154843</v>
-      </c>
+      <c r="C253" s="9"/>
+      <c r="D253" s="10"/>
+      <c r="E253" s="11"/>
+      <c r="F253" s="9"/>
+      <c r="G253" s="10"/>
+      <c r="H253" s="11"/>
       <c r="I253" s="9"/>
       <c r="J253" s="10"/>
       <c r="K253" s="11"/>
-      <c r="L253" s="9">
-        <v>143.96809164457954</v>
-      </c>
-      <c r="M253" s="10">
-        <v>121.68083427201414</v>
-      </c>
-      <c r="N253" s="11">
-        <v>139.95293223948315</v>
-      </c>
+      <c r="L253" s="9"/>
+      <c r="M253" s="10"/>
+      <c r="N253" s="11"/>
     </row>
     <row r="254" spans="3:14" ht="15">
-      <c r="C254" s="9">
-        <v>161.41687588300761</v>
-      </c>
-      <c r="D254" s="10">
-        <v>172.18528027317967</v>
-      </c>
-      <c r="E254" s="11">
-        <v>163.34536541463231</v>
-      </c>
-      <c r="F254" s="9">
-        <v>169.46661890038396</v>
-      </c>
-      <c r="G254" s="10">
-        <v>193.82317943515048</v>
-      </c>
-      <c r="H254" s="11">
-        <v>173.77981267319794</v>
-      </c>
+      <c r="C254" s="9"/>
+      <c r="D254" s="10"/>
+      <c r="E254" s="11"/>
+      <c r="F254" s="9"/>
+      <c r="G254" s="10"/>
+      <c r="H254" s="11"/>
       <c r="I254" s="9"/>
       <c r="J254" s="10"/>
       <c r="K254" s="11"/>
-      <c r="L254" s="9">
-        <v>144.12849354419839</v>
-      </c>
-      <c r="M254" s="10">
-        <v>120.97437620794983</v>
-      </c>
-      <c r="N254" s="11">
-        <v>139.93490408202121</v>
-      </c>
+      <c r="L254" s="9"/>
+      <c r="M254" s="10"/>
+      <c r="N254" s="11"/>
     </row>
     <row r="255" spans="3:14" ht="15">
-      <c r="C255" s="9">
-        <v>189.65200865533237</v>
-      </c>
-      <c r="D255" s="10">
-        <v>162.91283630865422</v>
-      </c>
-      <c r="E255" s="11">
-        <v>182.98060284111529</v>
-      </c>
-      <c r="F255" s="9">
-        <v>196.06789063054461</v>
-      </c>
-      <c r="G255" s="10">
-        <v>181.79372084545679</v>
-      </c>
-      <c r="H255" s="11">
-        <v>191.79434736168722</v>
-      </c>
+      <c r="C255" s="9"/>
+      <c r="D255" s="10"/>
+      <c r="E255" s="11"/>
+      <c r="F255" s="9"/>
+      <c r="G255" s="10"/>
+      <c r="H255" s="11"/>
       <c r="I255" s="9"/>
       <c r="J255" s="10"/>
       <c r="K255" s="11"/>
-      <c r="L255" s="9">
-        <v>158.80705308179503</v>
-      </c>
-      <c r="M255" s="10">
-        <v>121.64934121191398</v>
-      </c>
-      <c r="N255" s="11">
-        <v>152.30104529345678</v>
-      </c>
+      <c r="L255" s="9"/>
+      <c r="M255" s="10"/>
+      <c r="N255" s="11"/>
     </row>
     <row r="256" spans="3:14" ht="15">
-      <c r="C256" s="9">
-        <v>184.81839621081912</v>
-      </c>
-      <c r="D256" s="10">
-        <v>161.69540907848369</v>
-      </c>
-      <c r="E256" s="11">
-        <v>179.31172738400011</v>
-      </c>
-      <c r="F256" s="9">
-        <v>186.17060673045307</v>
-      </c>
-      <c r="G256" s="10">
-        <v>179.83761371066936</v>
-      </c>
-      <c r="H256" s="11">
-        <v>183.54314341221144</v>
-      </c>
+      <c r="C256" s="9"/>
+      <c r="D256" s="10"/>
+      <c r="E256" s="11"/>
+      <c r="F256" s="9"/>
+      <c r="G256" s="10"/>
+      <c r="H256" s="11"/>
       <c r="I256" s="9"/>
       <c r="J256" s="10"/>
       <c r="K256" s="11"/>
-      <c r="L256" s="9">
-        <v>149.50720878408498</v>
-      </c>
-      <c r="M256" s="10">
-        <v>120.66681290881458</v>
-      </c>
-      <c r="N256" s="11">
-        <v>144.78440779445404</v>
-      </c>
+      <c r="L256" s="9"/>
+      <c r="M256" s="10"/>
+      <c r="N256" s="11"/>
     </row>
     <row r="257" spans="3:14" ht="15">
-      <c r="C257" s="9">
-        <v>157.22218039227798</v>
-      </c>
-      <c r="D257" s="10">
-        <v>160.02895680592374</v>
-      </c>
-      <c r="E257" s="11">
-        <v>157.48131879057033</v>
-      </c>
-      <c r="F257" s="9">
-        <v>160.22979624437158</v>
-      </c>
-      <c r="G257" s="10">
-        <v>179.34050664430669</v>
-      </c>
-      <c r="H257" s="11">
-        <v>163.63637571642352</v>
-      </c>
+      <c r="C257" s="9"/>
+      <c r="D257" s="10"/>
+      <c r="E257" s="11"/>
+      <c r="F257" s="9"/>
+      <c r="G257" s="10"/>
+      <c r="H257" s="11"/>
       <c r="I257" s="9"/>
       <c r="J257" s="10"/>
       <c r="K257" s="11"/>
-      <c r="L257" s="9">
-        <v>129.45968169203289</v>
-      </c>
-      <c r="M257" s="10">
-        <v>110.62557699671464</v>
-      </c>
-      <c r="N257" s="11">
-        <v>126.3533505624343</v>
-      </c>
+      <c r="L257" s="9"/>
+      <c r="M257" s="10"/>
+      <c r="N257" s="11"/>
     </row>
     <row r="258" spans="3:14" ht="15">
-      <c r="C258" s="9">
-        <v>166.7934580471443</v>
-      </c>
-      <c r="D258" s="10">
-        <v>171.07317232700737</v>
-      </c>
-      <c r="E258" s="11">
-        <v>166.60309503188392</v>
-      </c>
-      <c r="F258" s="9">
-        <v>175.24077071509208</v>
-      </c>
-      <c r="G258" s="10">
-        <v>190.11555792777477</v>
-      </c>
-      <c r="H258" s="11">
-        <v>177.58651631274853</v>
-      </c>
+      <c r="C258" s="9"/>
+      <c r="D258" s="10"/>
+      <c r="E258" s="11"/>
+      <c r="F258" s="9"/>
+      <c r="G258" s="10"/>
+      <c r="H258" s="11"/>
       <c r="I258" s="9"/>
       <c r="J258" s="10"/>
       <c r="K258" s="11"/>
-      <c r="L258" s="9">
-        <v>138.14727204689123</v>
-      </c>
-      <c r="M258" s="10">
-        <v>122.91607766493431</v>
-      </c>
-      <c r="N258" s="11">
-        <v>135.29935332441798</v>
-      </c>
+      <c r="L258" s="9"/>
+      <c r="M258" s="10"/>
+      <c r="N258" s="11"/>
     </row>
     <row r="259" spans="3:14" ht="15">
-      <c r="C259" s="9">
-        <v>157.40192171954126</v>
-      </c>
-      <c r="D259" s="10">
-        <v>176.06704989241442</v>
-      </c>
-      <c r="E259" s="11">
-        <v>161.01532357927547</v>
-      </c>
-      <c r="F259" s="9">
-        <v>170.41040874793762</v>
-      </c>
-      <c r="G259" s="10">
-        <v>197.52351452396198</v>
-      </c>
-      <c r="H259" s="11">
-        <v>175.31130529462936</v>
-      </c>
+      <c r="C259" s="9"/>
+      <c r="D259" s="10"/>
+      <c r="E259" s="11"/>
+      <c r="F259" s="9"/>
+      <c r="G259" s="10"/>
+      <c r="H259" s="11"/>
       <c r="I259" s="9"/>
       <c r="J259" s="10"/>
       <c r="K259" s="11"/>
-      <c r="L259" s="9">
-        <v>135.53671105730831</v>
-      </c>
-      <c r="M259" s="10">
-        <v>116.87848462420986</v>
-      </c>
-      <c r="N259" s="11">
-        <v>132.40282479626458</v>
-      </c>
+      <c r="L259" s="9"/>
+      <c r="M259" s="10"/>
+      <c r="N259" s="11"/>
     </row>
     <row r="260" spans="3:14" ht="15">
-      <c r="C260" s="9">
-        <v>159.93763198124267</v>
-      </c>
-      <c r="D260" s="10">
-        <v>174.70522061784027</v>
-      </c>
-      <c r="E260" s="11">
-        <v>162.61547469893949</v>
-      </c>
-      <c r="F260" s="9">
-        <v>176.32198230249483</v>
-      </c>
-      <c r="G260" s="10">
-        <v>204.15277546828881</v>
-      </c>
-      <c r="H260" s="11">
-        <v>181.12679768294797</v>
-      </c>
+      <c r="C260" s="9"/>
+      <c r="D260" s="10"/>
+      <c r="E260" s="11"/>
+      <c r="F260" s="9"/>
+      <c r="G260" s="10"/>
+      <c r="H260" s="11"/>
       <c r="I260" s="9"/>
       <c r="J260" s="10"/>
       <c r="K260" s="11"/>
-      <c r="L260" s="9">
-        <v>143.58136558088063</v>
-      </c>
-      <c r="M260" s="10">
-        <v>124.09356698391258</v>
-      </c>
-      <c r="N260" s="11">
-        <v>140.52360742138004</v>
-      </c>
+      <c r="L260" s="9"/>
+      <c r="M260" s="10"/>
+      <c r="N260" s="11"/>
     </row>
     <row r="261" spans="3:14" ht="15">
-      <c r="C261" s="9">
-        <v>157.05472124709445</v>
-      </c>
-      <c r="D261" s="10">
-        <v>174.32520360030642</v>
-      </c>
-      <c r="E261" s="11">
-        <v>160.42910375171633</v>
-      </c>
-      <c r="F261" s="9">
-        <v>164.94961162158452</v>
-      </c>
-      <c r="G261" s="10">
-        <v>196.16347276587638</v>
-      </c>
-      <c r="H261" s="11">
-        <v>170.53142696078453</v>
-      </c>
+      <c r="C261" s="9"/>
+      <c r="D261" s="10"/>
+      <c r="E261" s="11"/>
+      <c r="F261" s="9"/>
+      <c r="G261" s="10"/>
+      <c r="H261" s="11"/>
       <c r="I261" s="9"/>
       <c r="J261" s="10"/>
       <c r="K261" s="11"/>
-      <c r="L261" s="9">
-        <v>139.20493713093879</v>
-      </c>
-      <c r="M261" s="10">
-        <v>119.27110026518969</v>
-      </c>
-      <c r="N261" s="11">
-        <v>135.4590354494855</v>
-      </c>
+      <c r="L261" s="9"/>
+      <c r="M261" s="10"/>
+      <c r="N261" s="11"/>
     </row>
     <row r="262" spans="3:14" ht="15">
-      <c r="C262" s="9">
-        <v>175.99035442524317</v>
-      </c>
-      <c r="D262" s="10">
-        <v>187.49407563892481</v>
-      </c>
-      <c r="E262" s="11">
-        <v>178.18402458118334</v>
-      </c>
-      <c r="F262" s="9">
-        <v>184.92253652723861</v>
-      </c>
-      <c r="G262" s="10">
-        <v>209.96477145083696</v>
-      </c>
-      <c r="H262" s="11">
-        <v>189.11080490900389</v>
-      </c>
+      <c r="C262" s="9"/>
+      <c r="D262" s="10"/>
+      <c r="E262" s="11"/>
+      <c r="F262" s="9"/>
+      <c r="G262" s="10"/>
+      <c r="H262" s="11"/>
       <c r="I262" s="9"/>
       <c r="J262" s="10"/>
       <c r="K262" s="11"/>
-      <c r="L262" s="9">
-        <v>157.53556674934242</v>
-      </c>
-      <c r="M262" s="10">
-        <v>133.01237078313753</v>
-      </c>
-      <c r="N262" s="11">
-        <v>153.28951490815004</v>
-      </c>
+      <c r="L262" s="9"/>
+      <c r="M262" s="10"/>
+      <c r="N262" s="11"/>
     </row>
     <row r="263" spans="3:14" ht="15">
-      <c r="C263" s="9">
-        <v>164.4291159354722</v>
-      </c>
-      <c r="D263" s="10">
-        <v>186.59576763484694</v>
-      </c>
-      <c r="E263" s="11">
-        <v>168.96287806990608</v>
-      </c>
-      <c r="F263" s="9">
-        <v>174.14423575542739</v>
-      </c>
-      <c r="G263" s="10">
-        <v>210.35055038549638</v>
-      </c>
-      <c r="H263" s="11">
-        <v>181.29934834508495</v>
-      </c>
+      <c r="C263" s="9"/>
+      <c r="D263" s="10"/>
+      <c r="E263" s="11"/>
+      <c r="F263" s="9"/>
+      <c r="G263" s="10"/>
+      <c r="H263" s="11"/>
       <c r="I263" s="9"/>
       <c r="J263" s="10"/>
       <c r="K263" s="11"/>
-      <c r="L263" s="9">
-        <v>143.07493296813891</v>
-      </c>
-      <c r="M263" s="10">
-        <v>128.45514443271443</v>
-      </c>
-      <c r="N263" s="11">
-        <v>140.52216242701471</v>
-      </c>
+      <c r="L263" s="9"/>
+      <c r="M263" s="10"/>
+      <c r="N263" s="11"/>
     </row>
     <row r="264" spans="3:14" ht="15">
-      <c r="C264" s="9">
-        <v>164.70492636130734</v>
-      </c>
-      <c r="D264" s="10">
-        <v>180.60678225383415</v>
-      </c>
-      <c r="E264" s="11">
-        <v>167.77993628539815</v>
-      </c>
-      <c r="F264" s="9">
-        <v>173.90207767458969</v>
-      </c>
-      <c r="G264" s="10">
-        <v>203.84957040949402</v>
-      </c>
-      <c r="H264" s="11">
-        <v>180.00416738829</v>
-      </c>
+      <c r="C264" s="9"/>
+      <c r="D264" s="10"/>
+      <c r="E264" s="11"/>
+      <c r="F264" s="9"/>
+      <c r="G264" s="10"/>
+      <c r="H264" s="11"/>
       <c r="I264" s="9"/>
       <c r="J264" s="10"/>
       <c r="K264" s="11"/>
-      <c r="L264" s="9">
-        <v>146.29957197876132</v>
-      </c>
-      <c r="M264" s="10">
-        <v>129.02762611183564</v>
-      </c>
-      <c r="N264" s="11">
-        <v>143.17964664598924</v>
-      </c>
+      <c r="L264" s="9"/>
+      <c r="M264" s="10"/>
+      <c r="N264" s="11"/>
     </row>
     <row r="265" spans="3:14" ht="15">
       <c r="C265" s="9">
@@ -13343,6 +12834,1938 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2836FE96-086E-134D-911E-50154836EBD7}">
+  <dimension ref="A2:D234"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="B2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>37622</v>
+      </c>
+      <c r="B5" s="5">
+        <v>99.999999999999972</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>37653</v>
+      </c>
+      <c r="B6" s="5">
+        <v>100.93161507068565</v>
+      </c>
+      <c r="C6" s="19">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>37681</v>
+      </c>
+      <c r="B7" s="5">
+        <v>101.27860547645155</v>
+      </c>
+      <c r="C7" s="19">
+        <v>100.9</v>
+      </c>
+      <c r="D7" s="19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>37712</v>
+      </c>
+      <c r="B8" s="5">
+        <v>100.64543904446134</v>
+      </c>
+      <c r="C8" s="20">
+        <v>101.3</v>
+      </c>
+      <c r="D8" s="20">
+        <v>100.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>37742</v>
+      </c>
+      <c r="B9" s="5">
+        <v>101.14416417496236</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20">
+        <v>101.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>37773</v>
+      </c>
+      <c r="B10" s="5">
+        <v>99.414657397942094</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20">
+        <v>100.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>37803</v>
+      </c>
+      <c r="B11" s="5">
+        <v>100.7646946126448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>37834</v>
+      </c>
+      <c r="B12" s="5">
+        <v>101.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>37865</v>
+      </c>
+      <c r="B13" s="5">
+        <v>103.91388184742408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>37895</v>
+      </c>
+      <c r="B14" s="5">
+        <v>105.02985824761916</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>37926</v>
+      </c>
+      <c r="B15" s="5">
+        <v>103.2855064498478</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>37956</v>
+      </c>
+      <c r="B16" s="5">
+        <v>102.87676275270746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>37987</v>
+      </c>
+      <c r="B17" s="5">
+        <v>103.09288954876487</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>38018</v>
+      </c>
+      <c r="B18" s="5">
+        <v>102.96727793699399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>38047</v>
+      </c>
+      <c r="B19" s="5">
+        <v>109.97112407844365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>38078</v>
+      </c>
+      <c r="B20" s="5">
+        <v>106.21289167756721</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>38108</v>
+      </c>
+      <c r="B21" s="5">
+        <v>107.24279138242052</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>38139</v>
+      </c>
+      <c r="B22" s="5">
+        <v>108.59655199542813</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>38169</v>
+      </c>
+      <c r="B23" s="5">
+        <v>110.33908513707553</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>38200</v>
+      </c>
+      <c r="B24" s="5">
+        <v>109.63153612752572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>38231</v>
+      </c>
+      <c r="B25" s="5">
+        <v>109.53938033578447</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>38261</v>
+      </c>
+      <c r="B26" s="5">
+        <v>108.43021452678046</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>38292</v>
+      </c>
+      <c r="B27" s="5">
+        <v>108.38741856152184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>38322</v>
+      </c>
+      <c r="B28" s="5">
+        <v>110.42221435264945</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>38353</v>
+      </c>
+      <c r="B29" s="5">
+        <v>108.25857901380255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>38384</v>
+      </c>
+      <c r="B30" s="5">
+        <v>106.47001620719486</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>38412</v>
+      </c>
+      <c r="B31" s="5">
+        <v>112.5317743729407</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>38443</v>
+      </c>
+      <c r="B32" s="5">
+        <v>110.81004056254775</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>38473</v>
+      </c>
+      <c r="B33" s="5">
+        <v>111.64944950543682</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>38504</v>
+      </c>
+      <c r="B34" s="5">
+        <v>112.81488851403688</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>38534</v>
+      </c>
+      <c r="B35" s="5">
+        <v>111.79916313868914</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>38565</v>
+      </c>
+      <c r="B36" s="5">
+        <v>113.63634430403143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>38596</v>
+      </c>
+      <c r="B37" s="5">
+        <v>112.03902735904929</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>38626</v>
+      </c>
+      <c r="B38" s="5">
+        <v>111.09018531471033</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>38657</v>
+      </c>
+      <c r="B39" s="5">
+        <v>111.97967118326939</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>38687</v>
+      </c>
+      <c r="B40" s="5">
+        <v>115.21553506640501</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>38718</v>
+      </c>
+      <c r="B41" s="5">
+        <v>113.25248300585885</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1">
+        <v>38749</v>
+      </c>
+      <c r="B42" s="5">
+        <v>109.72779353946542</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1">
+        <v>38777</v>
+      </c>
+      <c r="B43" s="5">
+        <v>114.58158997564104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1">
+        <v>38808</v>
+      </c>
+      <c r="B44" s="5">
+        <v>110.86084693615278</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1">
+        <v>38838</v>
+      </c>
+      <c r="B45" s="5">
+        <v>117.58712540682407</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1">
+        <v>38869</v>
+      </c>
+      <c r="B46" s="5">
+        <v>116.28416132891283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1">
+        <v>38899</v>
+      </c>
+      <c r="B47" s="5">
+        <v>117.85731402504931</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1">
+        <v>38930</v>
+      </c>
+      <c r="B48" s="5">
+        <v>119.45703768021045</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>38961</v>
+      </c>
+      <c r="B49" s="5">
+        <v>117.32502378535779</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
+        <v>38991</v>
+      </c>
+      <c r="B50" s="5">
+        <v>117.72931864714162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
+        <v>39022</v>
+      </c>
+      <c r="B51" s="5">
+        <v>117.89709393522583</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>39052</v>
+      </c>
+      <c r="B52" s="5">
+        <v>118.87192455431827</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>39083</v>
+      </c>
+      <c r="B53" s="5">
+        <v>118.52143567332266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>39114</v>
+      </c>
+      <c r="B54" s="5">
+        <v>113.92989247831312</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>39142</v>
+      </c>
+      <c r="B55" s="5">
+        <v>119.4826084631468</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>39173</v>
+      </c>
+      <c r="B56" s="5">
+        <v>116.99814395528425</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>39203</v>
+      </c>
+      <c r="B57" s="5">
+        <v>124.3054665742771</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>39234</v>
+      </c>
+      <c r="B58" s="5">
+        <v>123.85710852224176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>39264</v>
+      </c>
+      <c r="B59" s="5">
+        <v>125.83042665097288</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>39295</v>
+      </c>
+      <c r="B60" s="5">
+        <v>127.37055511882694</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>39326</v>
+      </c>
+      <c r="B61" s="5">
+        <v>124.37181470688934</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>39356</v>
+      </c>
+      <c r="B62" s="5">
+        <v>127.79432498473999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>39387</v>
+      </c>
+      <c r="B63" s="5">
+        <v>125.90988075748574</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>39417</v>
+      </c>
+      <c r="B64" s="5">
+        <v>126.16841582081076</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>39448</v>
+      </c>
+      <c r="B65" s="5">
+        <v>125.35742822732755</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>39479</v>
+      </c>
+      <c r="B66" s="5">
+        <v>124.13873955381939</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>39508</v>
+      </c>
+      <c r="B67" s="5">
+        <v>125.86165264935701</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>39539</v>
+      </c>
+      <c r="B68" s="5">
+        <v>126.32915754904437</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>39569</v>
+      </c>
+      <c r="B69" s="5">
+        <v>131.27527333182769</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>39600</v>
+      </c>
+      <c r="B70" s="5">
+        <v>133.25759896537107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>39630</v>
+      </c>
+      <c r="B71" s="5">
+        <v>135.77824963871018</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>39661</v>
+      </c>
+      <c r="B72" s="5">
+        <v>134.03998385643189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
+        <v>39692</v>
+      </c>
+      <c r="B73" s="5">
+        <v>134.83417738253118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
+        <v>39722</v>
+      </c>
+      <c r="B74" s="5">
+        <v>133.21564373949909</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
+        <v>39753</v>
+      </c>
+      <c r="B75" s="5">
+        <v>126.38825743338236</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
+        <v>39783</v>
+      </c>
+      <c r="B76" s="5">
+        <v>123.98987021104165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>39814</v>
+      </c>
+      <c r="B77" s="5">
+        <v>122.19516143376035</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>39845</v>
+      </c>
+      <c r="B78" s="5">
+        <v>119.53972826688401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>39873</v>
+      </c>
+      <c r="B79" s="5">
+        <v>125.89819918373607</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
+        <v>39904</v>
+      </c>
+      <c r="B80" s="5">
+        <v>122.61169292113136</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
+        <v>39934</v>
+      </c>
+      <c r="B81" s="5">
+        <v>127.47804455892627</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>39965</v>
+      </c>
+      <c r="B82" s="5">
+        <v>130.05873855872366</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>39995</v>
+      </c>
+      <c r="B83" s="5">
+        <v>130.58677699800862</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>40026</v>
+      </c>
+      <c r="B84" s="5">
+        <v>131.58287315864416</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>40057</v>
+      </c>
+      <c r="B85" s="5">
+        <v>133.94475486922934</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1">
+        <v>40087</v>
+      </c>
+      <c r="B86" s="5">
+        <v>133.89484810404832</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1">
+        <v>40118</v>
+      </c>
+      <c r="B87" s="5">
+        <v>132.16921299880312</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1">
+        <v>40148</v>
+      </c>
+      <c r="B88" s="5">
+        <v>134.94013705342545</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>40179</v>
+      </c>
+      <c r="B89" s="5">
+        <v>131.77007143128679</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1">
+        <v>40210</v>
+      </c>
+      <c r="B90" s="5">
+        <v>131.24172519241722</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1">
+        <v>40238</v>
+      </c>
+      <c r="B91" s="5">
+        <v>140.80416395554525</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>40269</v>
+      </c>
+      <c r="B92" s="5">
+        <v>135.15030050262999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>40299</v>
+      </c>
+      <c r="B93" s="5">
+        <v>139.04900368789831</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>40330</v>
+      </c>
+      <c r="B94" s="5">
+        <v>139.0928137419065</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>40360</v>
+      </c>
+      <c r="B95" s="5">
+        <v>140.42573961475293</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>40391</v>
+      </c>
+      <c r="B96" s="5">
+        <v>141.88690207026403</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>40422</v>
+      </c>
+      <c r="B97" s="5">
+        <v>141.92431033482904</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>40452</v>
+      </c>
+      <c r="B98" s="5">
+        <v>140.71659172067237</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>40483</v>
+      </c>
+      <c r="B99" s="5">
+        <v>141.79874094622826</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>40513</v>
+      </c>
+      <c r="B100" s="5">
+        <v>143.27339237476573</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>40544</v>
+      </c>
+      <c r="B101" s="5">
+        <v>138.87974539333217</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>40575</v>
+      </c>
+      <c r="B102" s="5">
+        <v>139.58216449739243</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>40603</v>
+      </c>
+      <c r="B103" s="5">
+        <v>141.29576427540755</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>40634</v>
+      </c>
+      <c r="B104" s="5">
+        <v>138.30820749943169</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>40664</v>
+      </c>
+      <c r="B105" s="5">
+        <v>146.12139052548909</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>40695</v>
+      </c>
+      <c r="B106" s="5">
+        <v>145.38336274165815</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>40725</v>
+      </c>
+      <c r="B107" s="5">
+        <v>145.86451002316508</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>40756</v>
+      </c>
+      <c r="B108" s="5">
+        <v>147.63722272003048</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>40787</v>
+      </c>
+      <c r="B109" s="5">
+        <v>146.23087380735853</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>40817</v>
+      </c>
+      <c r="B110" s="5">
+        <v>144.44868215797956</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>40848</v>
+      </c>
+      <c r="B111" s="5">
+        <v>144.857454578627</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>40878</v>
+      </c>
+      <c r="B112" s="5">
+        <v>146.64129037476417</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1">
+        <v>40909</v>
+      </c>
+      <c r="B113" s="5">
+        <v>140.57731185769384</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1">
+        <v>40940</v>
+      </c>
+      <c r="B114" s="5">
+        <v>140.07271766230764</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1">
+        <v>40969</v>
+      </c>
+      <c r="B115" s="5">
+        <v>143.8649960730786</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1">
+        <v>41000</v>
+      </c>
+      <c r="B116" s="5">
+        <v>139.20454908614852</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1">
+        <v>41030</v>
+      </c>
+      <c r="B117" s="5">
+        <v>148.54719383024701</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1">
+        <v>41061</v>
+      </c>
+      <c r="B118" s="5">
+        <v>148.41972868947551</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1">
+        <v>41091</v>
+      </c>
+      <c r="B119" s="5">
+        <v>150.16050089877984</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1">
+        <v>41122</v>
+      </c>
+      <c r="B120" s="5">
+        <v>153.4115086660253</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1">
+        <v>41153</v>
+      </c>
+      <c r="B121" s="5">
+        <v>147.39457206215684</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1">
+        <v>41183</v>
+      </c>
+      <c r="B122" s="5">
+        <v>151.98259254263056</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1">
+        <v>41214</v>
+      </c>
+      <c r="B123" s="5">
+        <v>148.26372667978904</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1">
+        <v>41244</v>
+      </c>
+      <c r="B124" s="5">
+        <v>147.19715079295258</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1">
+        <v>41275</v>
+      </c>
+      <c r="B125" s="5">
+        <v>147.75074069230311</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1">
+        <v>41306</v>
+      </c>
+      <c r="B126" s="5">
+        <v>143.45008036669029</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="1">
+        <v>41334</v>
+      </c>
+      <c r="B127" s="5">
+        <v>148.7277541237147</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="1">
+        <v>41365</v>
+      </c>
+      <c r="B128" s="5">
+        <v>150.40706564838538</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="1">
+        <v>41395</v>
+      </c>
+      <c r="B129" s="5">
+        <v>152.18170993971063</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="1">
+        <v>41426</v>
+      </c>
+      <c r="B130" s="5">
+        <v>150.595023307497</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="1">
+        <v>41456</v>
+      </c>
+      <c r="B131" s="5">
+        <v>153.79949781271404</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="1">
+        <v>41487</v>
+      </c>
+      <c r="B132" s="5">
+        <v>155.15074315541227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="1">
+        <v>41518</v>
+      </c>
+      <c r="B133" s="5">
+        <v>152.60703162758432</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="1">
+        <v>41548</v>
+      </c>
+      <c r="B134" s="5">
+        <v>155.04208881189103</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="1">
+        <v>41579</v>
+      </c>
+      <c r="B135" s="5">
+        <v>152.00071347161708</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="1">
+        <v>41609</v>
+      </c>
+      <c r="B136" s="5">
+        <v>148.79951628948118</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="1">
+        <v>41640</v>
+      </c>
+      <c r="B137" s="5">
+        <v>149.91784828370459</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="1">
+        <v>41671</v>
+      </c>
+      <c r="B138" s="5">
+        <v>148.37863708985859</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="1">
+        <v>41699</v>
+      </c>
+      <c r="B139" s="5">
+        <v>150.52599346080942</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1">
+        <v>41730</v>
+      </c>
+      <c r="B140" s="5">
+        <v>149.77582943045397</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="1">
+        <v>41760</v>
+      </c>
+      <c r="B141" s="5">
+        <v>153.05093679198131</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="1">
+        <v>41791</v>
+      </c>
+      <c r="B142" s="5">
+        <v>148.55820730503453</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="1">
+        <v>41821</v>
+      </c>
+      <c r="B143" s="5">
+        <v>152.26009978514045</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="1">
+        <v>41852</v>
+      </c>
+      <c r="B144" s="5">
+        <v>153.22972495927104</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="1">
+        <v>41883</v>
+      </c>
+      <c r="B145" s="5">
+        <v>152.61693565660241</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B146" s="5">
+        <v>154.43829192858999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="1">
+        <v>41944</v>
+      </c>
+      <c r="B147" s="5">
+        <v>150.1855612580201</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="1">
+        <v>41974</v>
+      </c>
+      <c r="B148" s="5">
+        <v>148.85193506366326</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B149" s="5">
+        <v>148.47107792296785</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B150" s="5">
+        <v>144.683414963334</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1">
+        <v>42064</v>
+      </c>
+      <c r="B151" s="3">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="1">
+        <v>42095</v>
+      </c>
+      <c r="B152" s="5">
+        <v>146.0285999806068</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="1">
+        <v>42125</v>
+      </c>
+      <c r="B153" s="5">
+        <v>147.41466537633261</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B154" s="5">
+        <v>146.4683352588174</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="1">
+        <v>42186</v>
+      </c>
+      <c r="B155" s="5">
+        <v>147.69587825713111</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="1">
+        <v>42217</v>
+      </c>
+      <c r="B156" s="5">
+        <v>148.01868108294076</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="1">
+        <v>42248</v>
+      </c>
+      <c r="B157" s="5">
+        <v>145.96275410405082</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="1">
+        <v>42278</v>
+      </c>
+      <c r="B158" s="5">
+        <v>147.31518267735788</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B159" s="5">
+        <v>143.05542053082891</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="1">
+        <v>42339</v>
+      </c>
+      <c r="B160" s="5">
+        <v>142.18277064387587</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B161" s="5">
+        <v>140.6308781065957</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B162" s="5">
+        <v>139.65749634389815</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="1">
+        <v>42430</v>
+      </c>
+      <c r="B163" s="5">
+        <v>143.36067320182755</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="1">
+        <v>42461</v>
+      </c>
+      <c r="B164" s="5">
+        <v>141.30335616118998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B165" s="5">
+        <v>142.66586636652025</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" s="1">
+        <v>42522</v>
+      </c>
+      <c r="B166" s="5">
+        <v>143.12310551008437</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B167" s="5">
+        <v>143.83146981838848</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B168" s="5">
+        <v>144.87821062242938</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B169" s="5">
+        <v>142.43328002334457</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B170" s="5">
+        <v>141.92819925716734</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B171" s="5">
+        <v>140.70396138644267</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B172" s="5">
+        <v>139.86955507532457</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B173" s="5">
+        <v>141.83924508122817</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" s="1">
+        <v>42767</v>
+      </c>
+      <c r="B174" s="5">
+        <v>139.12708578129039</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" s="1">
+        <v>42795</v>
+      </c>
+      <c r="B175" s="5">
+        <v>143.68772417119152</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B176" s="5">
+        <v>139.62273258219039</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" s="1">
+        <v>42856</v>
+      </c>
+      <c r="B177" s="5">
+        <v>144.52279577278449</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" s="1">
+        <v>42887</v>
+      </c>
+      <c r="B178" s="5">
+        <v>143.79013879261402</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" s="1">
+        <v>42917</v>
+      </c>
+      <c r="B179" s="5">
+        <v>144.86348521714015</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" s="1">
+        <v>42948</v>
+      </c>
+      <c r="B180" s="5">
+        <v>146.32218604027616</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" s="1">
+        <v>42979</v>
+      </c>
+      <c r="B181" s="5">
+        <v>144.09406845044776</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" s="1">
+        <v>43009</v>
+      </c>
+      <c r="B182" s="5">
+        <v>144.67619848002391</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" s="1">
+        <v>43040</v>
+      </c>
+      <c r="B183" s="5">
+        <v>143.17712839805799</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" s="1">
+        <v>43070</v>
+      </c>
+      <c r="B184" s="5">
+        <v>141.94439871741505</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B185" s="5">
+        <v>143.0616723003354</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B186" s="5">
+        <v>139.3671083496539</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B187" s="5">
+        <v>144.51186719480987</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" s="1">
+        <v>43191</v>
+      </c>
+      <c r="B188" s="5">
+        <v>143.74991117204712</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B189" s="5">
+        <v>142.64305895599475</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" s="1">
+        <v>43252</v>
+      </c>
+      <c r="B190" s="5">
+        <v>145.54104562430919</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B191" s="5">
+        <v>147.17745363035198</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" s="1">
+        <v>43313</v>
+      </c>
+      <c r="B192" s="5">
+        <v>149.02390894463551</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B193" s="5">
+        <v>144.86654099234488</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B194" s="5">
+        <v>147.15942710539403</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B195" s="5">
+        <v>144.86192079006045</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" s="1">
+        <v>43435</v>
+      </c>
+      <c r="B196" s="5">
+        <v>142.78193729337093</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B197" s="5">
+        <v>143.94102571183464</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B198" s="5">
+        <v>142.24011130694564</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" s="1">
+        <v>43525</v>
+      </c>
+      <c r="B199" s="5">
+        <v>143.36041202643648</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B200" s="5">
+        <v>143.97433994414661</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" s="1">
+        <v>43586</v>
+      </c>
+      <c r="B201" s="5">
+        <v>148.08282266052794</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B202" s="5">
+        <v>144.8886392477294</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" s="1">
+        <v>43647</v>
+      </c>
+      <c r="B203" s="5">
+        <v>148.58713785688104</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" s="1">
+        <v>43678</v>
+      </c>
+      <c r="B204" s="5">
+        <v>149.52057795494096</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" s="1">
+        <v>43709</v>
+      </c>
+      <c r="B205" s="5">
+        <v>147.17037871075092</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" s="1">
+        <v>43739</v>
+      </c>
+      <c r="B206" s="5">
+        <v>149.83448675949649</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B207" s="5">
+        <v>146.45447468638284</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B208" s="5">
+        <v>143.76797585061897</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B209" s="5">
+        <v>145.40578847591922</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B210" s="5">
+        <v>143.73844308813841</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B211" s="5">
+        <v>140.68803104386899</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B212" s="5">
+        <v>126.97455528348688</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B213" s="5">
+        <v>132.61911237523455</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B214" s="5">
+        <v>137.07460920361751</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B215" s="5">
+        <v>143.30930483918922</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B216" s="5">
+        <v>145.30336167974414</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B217" s="5">
+        <v>146.34923628145057</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" customFormat="1" ht="15">
+      <c r="A218" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B218" s="5">
+        <v>148.38144538534561</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B219" s="5">
+        <v>145.81658113318431</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B220" s="5">
+        <v>145.22848692870522</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B221" s="5">
+        <v>145.89215599423341</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B222" s="5">
+        <v>143.81268424157577</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B223" s="5">
+        <v>146.11401122646063</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B224" s="5">
+        <v>143.43813943592588</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B225" s="5">
+        <v>147.64459356005983</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B226" s="5">
+        <v>147.57357417071361</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B227" s="5">
+        <v>149.90117844989612</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B228" s="5">
+        <v>149.12075733244424</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B229" s="5">
+        <v>147.52466503492849</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B230" s="5">
+        <v>146.93508906857929</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B231" s="5">
+        <v>146.60902167549582</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B232" s="5">
+        <v>146.84026886309351</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;9&amp;K000000Corporativo | Interno</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B524F9-E8ED-E741-AD5C-9A2F061518E5}">
   <dimension ref="H8:I15"/>
   <sheetViews>
@@ -13413,6 +14836,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a958aac7-9816-4b49-a369-ffb0414a5901" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b9caf5d9-17e9-4d21-9144-efe8bc0590c0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041D011F16168614CB0D253271BB45155" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e62644e25f9d6041c9f704c224d0f0c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b9caf5d9-17e9-4d21-9144-efe8bc0590c0" xmlns:ns3="a958aac7-9816-4b49-a369-ffb0414a5901" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c19f748cb8524a99107a6cfe2d61b01" ns2:_="" ns3:_="">
     <xsd:import namespace="b9caf5d9-17e9-4d21-9144-efe8bc0590c0"/>
@@ -13607,34 +15050,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a958aac7-9816-4b49-a369-ffb0414a5901" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b9caf5d9-17e9-4d21-9144-efe8bc0590c0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0425180-5A32-4C8E-A38A-3E6434BAECD5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5121C8E2-EDC2-407B-926F-E6D2DD41FEA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a958aac7-9816-4b49-a369-ffb0414a5901"/>
+    <ds:schemaRef ds:uri="b9caf5d9-17e9-4d21-9144-efe8bc0590c0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E879C567-AEC0-4A11-9354-F262EE83727B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E879C567-AEC0-4A11-9354-F262EE83727B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5121C8E2-EDC2-407B-926F-E6D2DD41FEA8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0425180-5A32-4C8E-A38A-3E6434BAECD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b9caf5d9-17e9-4d21-9144-efe8bc0590c0"/>
+    <ds:schemaRef ds:uri="a958aac7-9816-4b49-a369-ffb0414a5901"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>